<commit_message>
adding 91 country code on numbers
Since filling out a google form or storing in an excel sheet, people tend to not write their county code, the program is optimized in a way to add the Indian Dialing code 91 on its own.
</commit_message>
<xml_diff>
--- a/Recipients data.xlsx
+++ b/Recipients data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB79466-0722-43D9-A219-66522859284C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115A68BB-BD9A-467F-8435-467F78011154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,27 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Message</t>
   </si>
   <si>
     <t>Contact</t>
-  </si>
-  <si>
-    <t>Hello Aryan, I obtained your contact information through Bangalore Tech Summit.          |           My name is Tapan and  I represent Akriti Precision Systems, manufacturer of the WORLD's 1st COMPOSITE SUPERSTRUCTURE 3-AXIS CNC MACHINE.                                           100% MADE IN INDIA                                   ZERO Chinese Parts                                    - 70% parts by value are sources from India and the rest from Italy Germany Taiwan Japan and Thailand           |             Product  Technical Specifications Video - https://www.youtube.com/watch?v=iC9diy4BY7w            |             Call or Whatsapp us on +919019054837 or email us on contact@akriti.tech to know more              |                 1 Year - Manufacturers Warranty (All Parts)           |             10 Years - Composite SuperStructure (Custom made by us)             |               Extended Warranty options also available           |              Perfect Machine for Wood MDF Acrylic Plastics with 50 MICRONS REPEAT POSITIONING ACCURACY             |                Soft Metals till Machine grade aluminium   Hard Materials like Granite   Glass can also be milled with an upgrade to a Double Bearing Spindle - Read More - https://akriti.tech/mighty</t>
-  </si>
-  <si>
-    <t>Hello Arshia, I obtained your contact information through Bangalore Tech Summit.          |           My name is Tapan and  I represent Akriti Precision Systems, manufacturer of the WORLD's 1st COMPOSITE SUPERSTRUCTURE 3-AXIS CNC MACHINE.                                           100% MADE IN INDIA                                   ZERO Chinese Parts                                    - 70% parts by value are sources from India and the rest from Italy Germany Taiwan Japan and Thailand           |             Product  Technical Specifications Video - https://www.youtube.com/watch?v=iC9diy4BY7w            |             Call or Whatsapp us on +919019054837 or email us on contact@akriti.tech to know more              |                 1 Year - Manufacturers Warranty (All Parts)           |             10 Years - Composite SuperStructure (Custom made by us)             |               Extended Warranty options also available           |              Perfect Machine for Wood MDF Acrylic Plastics with 50 MICRONS REPEAT POSITIONING ACCURACY             |                Soft Metals till Machine grade aluminium   Hard Materials like Granite   Glass can also be milled with an upgrade to a Double Bearing Spindle - Read More - https://akriti.tech/mighty</t>
-  </si>
-  <si>
-    <t>Hello Sanskar, I obtained your contact information through Bangalore Tech Summit.          |           My name is Tapan and  I represent Akriti Precision Systems, manufacturer of the WORLD's 1st COMPOSITE SUPERSTRUCTURE 3-AXIS CNC MACHINE.                                           100% MADE IN INDIA                                   ZERO Chinese Parts                                    - 70% parts by value are sources from India and the rest from Italy Germany Taiwan Japan and Thailand           |             Product  Technical Specifications Video - https://www.youtube.com/watch?v=iC9diy4BY7w            |             Call or Whatsapp us on +919019054837 or email us on contact@akriti.tech to know more              |                 1 Year - Manufacturers Warranty (All Parts)           |             10 Years - Composite SuperStructure (Custom made by us)             |               Extended Warranty options also available           |              Perfect Machine for Wood MDF Acrylic Plastics with 50 MICRONS REPEAT POSITIONING ACCURACY             |                Soft Metals till Machine grade aluminium   Hard Materials like Granite   Glass can also be milled with an upgrade to a Double Bearing Spindle - Read More - https://akriti.tech/mighty</t>
-  </si>
-  <si>
-    <t>Hello Shruti, I obtained your contact information through Bangalore Tech Summit.          |           My name is Tapan and  I represent Akriti Precision Systems, manufacturer of the WORLD's 1st COMPOSITE SUPERSTRUCTURE 3-AXIS CNC MACHINE.                                           100% MADE IN INDIA                                   ZERO Chinese Parts                                    - 70% parts by value are sources from India and the rest from Italy Germany Taiwan Japan and Thailand           |             Product  Technical Specifications Video - https://www.youtube.com/watch?v=iC9diy4BY7w            |             Call or Whatsapp us on +919019054837 or email us on contact@akriti.tech to know more              |                 1 Year - Manufacturers Warranty (All Parts)           |             10 Years - Composite SuperStructure (Custom made by us)             |               Extended Warranty options also available           |              Perfect Machine for Wood MDF Acrylic Plastics with 50 MICRONS REPEAT POSITIONING ACCURACY             |                Soft Metals till Machine grade aluminium   Hard Materials like Granite   Glass can also be milled with an upgrade to a Double Bearing Spindle - Read More - https://akriti.tech/mighty</t>
-  </si>
-  <si>
-    <t>Hello Shrishty, I obtained your contact information through Bangalore Tech Summit.          |           My name is Tapan and  I represent Akriti Precision Systems, manufacturer of the WORLD's 1st COMPOSITE SUPERSTRUCTURE 3-AXIS CNC MACHINE.                                           100% MADE IN INDIA                                   ZERO Chinese Parts                                    - 70% parts by value are sources from India and the rest from Italy Germany Taiwan Japan and Thailand           |             Product  Technical Specifications Video - https://www.youtube.com/watch?v=iC9diy4BY7w            |             Call or Whatsapp us on +919019054837 or email us on contact@akriti.tech to know more              |                 1 Year - Manufacturers Warranty (All Parts)           |             10 Years - Composite SuperStructure (Custom made by us)             |               Extended Warranty options also available           |              Perfect Machine for Wood MDF Acrylic Plastics with 50 MICRONS REPEAT POSITIONING ACCURACY             |                Soft Metals till Machine grade aluminium   Hard Materials like Granite   Glass can also be milled with an upgrade to a Double Bearing Spindle - Read More - https://akriti.tech/mighty</t>
   </si>
   <si>
     <t>Name</t>
@@ -166,6 +151,15 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <sz val="9"/>
         <color rgb="FF202124"/>
@@ -187,15 +181,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -273,16 +258,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B422" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Contact" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{EDAB1C5D-DC78-46F4-93F8-E5728DA2025C}" name="Name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{EDAB1C5D-DC78-46F4-93F8-E5728DA2025C}" name="Name" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="C1:C6" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="C1:C6" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Message" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Message" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -612,7 +597,7 @@
   <dimension ref="A1:C10644"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,66 +611,55 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>919910939598</v>
+        <v>9910939598</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>918383891488</v>
+        <v>8383891488</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>919868910520</v>
+        <v>9868910520</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>919319791269</v>
+        <v>9319791269</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>919599156056</v>
+        <v>9599156056</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>

</xml_diff>

<commit_message>
factoring files into folders
</commit_message>
<xml_diff>
--- a/Recipients data.xlsx
+++ b/Recipients data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84CC33B-28D4-4967-85BA-B1F6DBDCB4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4313F1-4D12-473A-BCAA-9A99575055BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="8">
   <si>
     <t>Message</t>
   </si>
@@ -35,7 +35,19 @@
     <t>Name</t>
   </si>
   <si>
-    <t>xyz</t>
+    <t>Aryan</t>
+  </si>
+  <si>
+    <t>Arshia</t>
+  </si>
+  <si>
+    <t>Sanskar</t>
+  </si>
+  <si>
+    <t>Shruti</t>
+  </si>
+  <si>
+    <t>Shrishty</t>
   </si>
 </sst>
 </file>
@@ -584,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10644"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +619,7 @@
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>9999999999</v>
+        <v>9910939598</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
@@ -615,339 +627,639 @@
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>9999999999</v>
+        <v>8383891488</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>9999999999</v>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>8383891488</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>9999999999</v>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>8383891488</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>9999999999</v>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>8383891488</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B18" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="5">
+        <v>9910939598</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="5">
+        <v>8383891488</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="5">
+        <v>9868910520</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="5">
+        <v>9319791269</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="5">
+        <v>9599156056</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>

</xml_diff>